<commit_message>
fixed hyperlink export, added layout info to excel export
</commit_message>
<xml_diff>
--- a/jobs/templates/Auswertung Untersuchungskriterien.xlsx
+++ b/jobs/templates/Auswertung Untersuchungskriterien.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D99668A-B206-4F3F-852C-4E2832B43A39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951B0F70-1920-4CA9-89D2-C6A311037201}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -487,35 +486,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -795,18 +797,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DA350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="AD21" sqref="AD21"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="77" max="77" width="8.85546875" style="10"/>
-    <col min="79" max="79" width="8.85546875" style="10"/>
-    <col min="81" max="81" width="8.85546875" style="10"/>
+    <col min="2" max="76" width="8.85546875" style="24"/>
+    <col min="77" max="77" width="8.85546875" style="25"/>
+    <col min="78" max="78" width="8.85546875" style="24"/>
+    <col min="79" max="79" width="8.85546875" style="25"/>
+    <col min="80" max="80" width="8.85546875" style="24"/>
+    <col min="81" max="81" width="8.85546875" style="25"/>
+    <col min="82" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:105" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -835,7 +841,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:105" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:105" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1123,10 +1129,10 @@
       <c r="CY2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="CZ2" s="11"/>
-      <c r="DA2" s="11"/>
-    </row>
-    <row r="3" spans="1:105" x14ac:dyDescent="0.25">
+      <c r="CZ2" s="10"/>
+      <c r="DA2" s="10"/>
+    </row>
+    <row r="3" spans="1:105" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1378,16 +1384,16 @@
       <c r="CK3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CL3" s="15" t="s">
+      <c r="CL3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="CM3" s="15" t="s">
+      <c r="CM3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="CN3" s="15" t="s">
+      <c r="CN3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="CO3" s="15" t="s">
+      <c r="CO3" s="14" t="s">
         <v>97</v>
       </c>
       <c r="CR3" s="3" t="s">
@@ -1414,8 +1420,8 @@
       <c r="CY3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CZ3" s="11"/>
-      <c r="DA3" s="11"/>
+      <c r="CZ3" s="10"/>
+      <c r="DA3" s="10"/>
     </row>
     <row r="4" spans="1:105" s="6" customFormat="1" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -1538,7 +1544,7 @@
       <c r="AN4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AO4" s="12" t="s">
+      <c r="AO4" s="11" t="s">
         <v>48</v>
       </c>
       <c r="AP4" s="4" t="s">
@@ -1646,25 +1652,25 @@
       <c r="BX4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BY4" s="13" t="s">
+      <c r="BY4" s="12" t="s">
         <v>87</v>
       </c>
       <c r="BZ4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="CA4" s="13" t="s">
+      <c r="CA4" s="12" t="s">
         <v>86</v>
       </c>
       <c r="CB4" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="CC4" s="13" t="s">
+      <c r="CC4" s="12" t="s">
         <v>92</v>
       </c>
       <c r="CD4" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CE4" s="13" t="s">
+      <c r="CE4" s="12" t="s">
         <v>93</v>
       </c>
       <c r="CF4" s="4" t="s">
@@ -1682,7 +1688,7 @@
       <c r="CJ4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CK4" s="14" t="s">
+      <c r="CK4" s="13" t="s">
         <v>91</v>
       </c>
       <c r="CL4" s="4" t="s">
@@ -1697,2842 +1703,2833 @@
       <c r="CO4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="CR4" s="14" t="s">
+      <c r="CR4" s="13" t="s">
         <v>102</v>
       </c>
       <c r="CS4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CT4" s="14" t="s">
+      <c r="CT4" s="13" t="s">
         <v>104</v>
       </c>
       <c r="CU4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CV4" s="14" t="s">
+      <c r="CV4" s="13" t="s">
         <v>105</v>
       </c>
       <c r="CW4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CX4" s="14" t="s">
+      <c r="CX4" s="13" t="s">
         <v>106</v>
       </c>
       <c r="CY4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="CZ4" s="16"/>
-      <c r="DA4" s="16"/>
-    </row>
-    <row r="5" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="CZ4" s="15"/>
+      <c r="DA4" s="15"/>
+    </row>
+    <row r="5" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
         <v>1</v>
       </c>
-      <c r="V5" s="21"/>
-      <c r="BK5" s="18"/>
-      <c r="BL5" s="18"/>
-      <c r="BM5" s="18"/>
-      <c r="BN5" s="18"/>
-      <c r="BO5" s="18"/>
-      <c r="BP5" s="18"/>
-      <c r="BQ5" s="18"/>
-      <c r="BR5" s="18"/>
-      <c r="BS5" s="18"/>
-      <c r="BT5" s="18"/>
-      <c r="BU5" s="18"/>
-      <c r="BV5" s="18"/>
-      <c r="BW5" s="18"/>
-      <c r="BX5" s="18"/>
-      <c r="BY5" s="19"/>
-      <c r="BZ5" s="18"/>
-      <c r="CA5" s="19"/>
-      <c r="CB5" s="18"/>
-      <c r="CC5" s="19"/>
-      <c r="CF5" s="18"/>
-      <c r="CG5" s="18"/>
-      <c r="CH5" s="18"/>
-      <c r="CI5" s="18"/>
-      <c r="CJ5" s="18"/>
-      <c r="CK5" s="18"/>
-      <c r="CM5" s="18"/>
-      <c r="CN5" s="18"/>
-    </row>
-    <row r="6" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="V5" s="18"/>
+      <c r="BK5" s="19"/>
+      <c r="BL5" s="19"/>
+      <c r="BM5" s="19"/>
+      <c r="BN5" s="19"/>
+      <c r="BO5" s="19"/>
+      <c r="BP5" s="19"/>
+      <c r="BQ5" s="19"/>
+      <c r="BR5" s="19"/>
+      <c r="BS5" s="19"/>
+      <c r="BT5" s="19"/>
+      <c r="BU5" s="19"/>
+      <c r="BV5" s="19"/>
+      <c r="BW5" s="19"/>
+      <c r="BX5" s="19"/>
+      <c r="BY5" s="20"/>
+      <c r="BZ5" s="19"/>
+      <c r="CA5" s="20"/>
+      <c r="CB5" s="19"/>
+      <c r="CC5" s="20"/>
+      <c r="CF5" s="19"/>
+      <c r="CG5" s="19"/>
+      <c r="CH5" s="19"/>
+      <c r="CI5" s="19"/>
+      <c r="CJ5" s="19"/>
+      <c r="CK5" s="19"/>
+      <c r="CM5" s="19"/>
+      <c r="CN5" s="19"/>
+    </row>
+    <row r="6" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
         <v>2</v>
       </c>
-      <c r="BW6" s="23"/>
+      <c r="BW6" s="21"/>
       <c r="BY6" s="22"/>
       <c r="CA6" s="22"/>
       <c r="CC6" s="22"/>
     </row>
-    <row r="7" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+    <row r="7" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
-      <c r="N7" s="24"/>
-      <c r="V7" s="25"/>
+      <c r="V7" s="23"/>
       <c r="BY7" s="22"/>
       <c r="CA7" s="22"/>
       <c r="CC7" s="22"/>
     </row>
-    <row r="8" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>4</v>
-      </c>
-      <c r="N8" s="24"/>
-      <c r="AE8" s="25"/>
+    <row r="8" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>4</v>
+      </c>
+      <c r="AE8" s="23"/>
       <c r="BY8" s="22"/>
       <c r="CA8" s="22"/>
       <c r="CC8" s="22"/>
     </row>
-    <row r="9" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+    <row r="9" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>5</v>
       </c>
-      <c r="N9" s="24"/>
-      <c r="V9" s="25"/>
+      <c r="V9" s="23"/>
       <c r="AM9" s="22"/>
       <c r="BY9" s="22"/>
       <c r="CA9" s="22"/>
       <c r="CC9" s="22"/>
     </row>
-    <row r="10" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
+    <row r="10" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>6</v>
       </c>
-      <c r="N10" s="24"/>
-      <c r="AE10" s="25"/>
+      <c r="AE10" s="23"/>
       <c r="BY10" s="22"/>
       <c r="CA10" s="22"/>
       <c r="CC10" s="22"/>
     </row>
-    <row r="11" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+    <row r="11" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
         <v>7</v>
       </c>
-      <c r="V11" s="25"/>
-      <c r="AM11" s="25"/>
+      <c r="V11" s="23"/>
+      <c r="AM11" s="23"/>
       <c r="BY11" s="22"/>
       <c r="CA11" s="22"/>
       <c r="CC11" s="22"/>
     </row>
-    <row r="12" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
+    <row r="12" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
         <v>8</v>
       </c>
-      <c r="N12" s="24"/>
-      <c r="AE12" s="25"/>
+      <c r="AE12" s="23"/>
       <c r="BY12" s="22"/>
       <c r="CA12" s="22"/>
       <c r="CC12" s="22"/>
     </row>
-    <row r="13" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
+    <row r="13" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
         <v>9</v>
       </c>
-      <c r="V13" s="25"/>
+      <c r="V13" s="23"/>
       <c r="BY13" s="22"/>
       <c r="CA13" s="22"/>
       <c r="CC13" s="22"/>
     </row>
-    <row r="14" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+    <row r="14" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>10</v>
       </c>
-      <c r="N14" s="24"/>
-      <c r="AE14" s="25"/>
+      <c r="AE14" s="23"/>
       <c r="BY14" s="22"/>
       <c r="CA14" s="22"/>
       <c r="CC14" s="22"/>
     </row>
-    <row r="15" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+    <row r="15" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>11</v>
       </c>
       <c r="BY15" s="22"/>
       <c r="CA15" s="22"/>
       <c r="CC15" s="22"/>
     </row>
-    <row r="16" spans="1:105" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
+    <row r="16" spans="1:105" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>12</v>
       </c>
-      <c r="N16" s="24"/>
-      <c r="AE16" s="21"/>
+      <c r="AE16" s="18"/>
       <c r="BY16" s="22"/>
       <c r="CA16" s="22"/>
       <c r="CC16" s="22"/>
     </row>
-    <row r="17" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
+    <row r="17" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16">
         <v>13</v>
       </c>
       <c r="BY17" s="22"/>
       <c r="CA17" s="22"/>
       <c r="CC17" s="22"/>
     </row>
-    <row r="18" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+    <row r="18" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
         <v>14</v>
       </c>
-      <c r="N18" s="24"/>
       <c r="BY18" s="22"/>
       <c r="CA18" s="22"/>
       <c r="CC18" s="22"/>
     </row>
-    <row r="19" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+    <row r="19" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>15</v>
       </c>
-      <c r="N19" s="24"/>
       <c r="BY19" s="22"/>
       <c r="CA19" s="22"/>
       <c r="CC19" s="22"/>
     </row>
-    <row r="20" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+    <row r="20" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
         <v>16</v>
       </c>
       <c r="BY20" s="22"/>
       <c r="CA20" s="22"/>
       <c r="CC20" s="22"/>
     </row>
-    <row r="21" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+    <row r="21" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
         <v>17</v>
       </c>
-      <c r="N21" s="25"/>
+      <c r="N21" s="23"/>
       <c r="BY21" s="22"/>
       <c r="CA21" s="22"/>
       <c r="CC21" s="22"/>
     </row>
-    <row r="22" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+    <row r="22" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
         <v>18</v>
       </c>
       <c r="BY22" s="22"/>
       <c r="CA22" s="22"/>
       <c r="CC22" s="22"/>
     </row>
-    <row r="23" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+    <row r="23" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
         <v>19</v>
       </c>
       <c r="BY23" s="22"/>
       <c r="CA23" s="22"/>
       <c r="CC23" s="22"/>
     </row>
-    <row r="24" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+    <row r="24" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
         <v>20</v>
       </c>
       <c r="BY24" s="22"/>
       <c r="CA24" s="22"/>
       <c r="CC24" s="22"/>
     </row>
-    <row r="25" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+    <row r="25" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16">
         <v>21</v>
       </c>
       <c r="BY25" s="22"/>
       <c r="CA25" s="22"/>
       <c r="CC25" s="22"/>
     </row>
-    <row r="26" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+    <row r="26" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
         <v>22</v>
       </c>
       <c r="BY26" s="22"/>
       <c r="CA26" s="22"/>
       <c r="CC26" s="22"/>
     </row>
-    <row r="27" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+    <row r="27" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16">
         <v>23</v>
       </c>
       <c r="BY27" s="22"/>
       <c r="CA27" s="22"/>
       <c r="CC27" s="22"/>
     </row>
-    <row r="28" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+    <row r="28" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
         <v>24</v>
       </c>
       <c r="BY28" s="22"/>
       <c r="CA28" s="22"/>
       <c r="CC28" s="22"/>
     </row>
-    <row r="29" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+    <row r="29" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
         <v>25</v>
       </c>
       <c r="BY29" s="22"/>
       <c r="CA29" s="22"/>
       <c r="CC29" s="22"/>
     </row>
-    <row r="30" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+    <row r="30" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="16">
         <v>26</v>
       </c>
       <c r="BY30" s="22"/>
       <c r="CA30" s="22"/>
       <c r="CC30" s="22"/>
     </row>
-    <row r="31" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+    <row r="31" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
         <v>27</v>
       </c>
       <c r="BY31" s="22"/>
       <c r="CA31" s="22"/>
       <c r="CC31" s="22"/>
     </row>
-    <row r="32" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+    <row r="32" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <v>28</v>
       </c>
       <c r="BY32" s="22"/>
       <c r="CA32" s="22"/>
       <c r="CC32" s="22"/>
     </row>
-    <row r="33" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
+    <row r="33" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
         <v>29</v>
       </c>
       <c r="BY33" s="22"/>
       <c r="CA33" s="22"/>
       <c r="CC33" s="22"/>
     </row>
-    <row r="34" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
+    <row r="34" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
         <v>30</v>
       </c>
       <c r="BY34" s="22"/>
       <c r="CA34" s="22"/>
       <c r="CC34" s="22"/>
     </row>
-    <row r="35" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+    <row r="35" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
         <v>31</v>
       </c>
       <c r="BY35" s="22"/>
       <c r="CA35" s="22"/>
       <c r="CC35" s="22"/>
     </row>
-    <row r="36" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+    <row r="36" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
         <v>32</v>
       </c>
       <c r="BY36" s="22"/>
       <c r="CA36" s="22"/>
       <c r="CC36" s="22"/>
     </row>
-    <row r="37" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
+    <row r="37" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
         <v>33</v>
       </c>
       <c r="BY37" s="22"/>
       <c r="CA37" s="22"/>
       <c r="CC37" s="22"/>
     </row>
-    <row r="38" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
+    <row r="38" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="16">
         <v>34</v>
       </c>
       <c r="BY38" s="22"/>
       <c r="CA38" s="22"/>
       <c r="CC38" s="22"/>
     </row>
-    <row r="39" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
+    <row r="39" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16">
         <v>35</v>
       </c>
       <c r="BY39" s="22"/>
       <c r="CA39" s="22"/>
       <c r="CC39" s="22"/>
     </row>
-    <row r="40" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
+    <row r="40" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="16">
         <v>36</v>
       </c>
       <c r="BY40" s="22"/>
       <c r="CA40" s="22"/>
       <c r="CC40" s="22"/>
     </row>
-    <row r="41" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
+    <row r="41" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16">
         <v>37</v>
       </c>
       <c r="BY41" s="22"/>
       <c r="CA41" s="22"/>
       <c r="CC41" s="22"/>
     </row>
-    <row r="42" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
+    <row r="42" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="16">
         <v>38</v>
       </c>
       <c r="BY42" s="22"/>
       <c r="CA42" s="22"/>
       <c r="CC42" s="22"/>
     </row>
-    <row r="43" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
+    <row r="43" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16">
         <v>39</v>
       </c>
       <c r="BY43" s="22"/>
       <c r="CA43" s="22"/>
       <c r="CC43" s="22"/>
     </row>
-    <row r="44" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
+    <row r="44" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="16">
         <v>40</v>
       </c>
       <c r="BY44" s="22"/>
       <c r="CA44" s="22"/>
       <c r="CC44" s="22"/>
     </row>
-    <row r="45" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
+    <row r="45" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
         <v>41</v>
       </c>
       <c r="BY45" s="22"/>
       <c r="CA45" s="22"/>
       <c r="CC45" s="22"/>
     </row>
-    <row r="46" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
+    <row r="46" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="16">
         <v>42</v>
       </c>
       <c r="BY46" s="22"/>
       <c r="CA46" s="22"/>
       <c r="CC46" s="22"/>
     </row>
-    <row r="47" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
+    <row r="47" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="16">
         <v>43</v>
       </c>
       <c r="BY47" s="22"/>
       <c r="CA47" s="22"/>
       <c r="CC47" s="22"/>
     </row>
-    <row r="48" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
+    <row r="48" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="16">
         <v>44</v>
       </c>
       <c r="BY48" s="22"/>
       <c r="CA48" s="22"/>
       <c r="CC48" s="22"/>
     </row>
-    <row r="49" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
+    <row r="49" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="16">
         <v>45</v>
       </c>
       <c r="BY49" s="22"/>
       <c r="CA49" s="22"/>
       <c r="CC49" s="22"/>
     </row>
-    <row r="50" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
+    <row r="50" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="16">
         <v>46</v>
       </c>
       <c r="BY50" s="22"/>
       <c r="CA50" s="22"/>
       <c r="CC50" s="22"/>
     </row>
-    <row r="51" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
+    <row r="51" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="16">
         <v>47</v>
       </c>
       <c r="BY51" s="22"/>
       <c r="CA51" s="22"/>
       <c r="CC51" s="22"/>
     </row>
-    <row r="52" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
+    <row r="52" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
         <v>48</v>
       </c>
       <c r="BY52" s="22"/>
       <c r="CA52" s="22"/>
       <c r="CC52" s="22"/>
     </row>
-    <row r="53" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
+    <row r="53" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="16">
         <v>49</v>
       </c>
       <c r="BY53" s="22"/>
       <c r="CA53" s="22"/>
       <c r="CC53" s="22"/>
     </row>
-    <row r="54" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
+    <row r="54" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="16">
         <v>50</v>
       </c>
       <c r="BY54" s="22"/>
       <c r="CA54" s="22"/>
       <c r="CC54" s="22"/>
     </row>
-    <row r="55" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
+    <row r="55" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
         <v>51</v>
       </c>
       <c r="BY55" s="22"/>
       <c r="CA55" s="22"/>
       <c r="CC55" s="22"/>
     </row>
-    <row r="56" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
+    <row r="56" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
         <v>52</v>
       </c>
       <c r="BY56" s="22"/>
       <c r="CA56" s="22"/>
       <c r="CC56" s="22"/>
     </row>
-    <row r="57" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
+    <row r="57" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
         <v>53</v>
       </c>
       <c r="BY57" s="22"/>
       <c r="CA57" s="22"/>
       <c r="CC57" s="22"/>
     </row>
-    <row r="58" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
+    <row r="58" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="16">
         <v>54</v>
       </c>
       <c r="BY58" s="22"/>
       <c r="CA58" s="22"/>
       <c r="CC58" s="22"/>
     </row>
-    <row r="59" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+    <row r="59" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="16">
         <v>55</v>
       </c>
       <c r="BY59" s="22"/>
       <c r="CA59" s="22"/>
       <c r="CC59" s="22"/>
     </row>
-    <row r="60" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
+    <row r="60" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="16">
         <v>56</v>
       </c>
       <c r="BY60" s="22"/>
       <c r="CA60" s="22"/>
       <c r="CC60" s="22"/>
     </row>
-    <row r="61" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
+    <row r="61" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="16">
         <v>57</v>
       </c>
       <c r="BY61" s="22"/>
       <c r="CA61" s="22"/>
       <c r="CC61" s="22"/>
     </row>
-    <row r="62" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
+    <row r="62" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="16">
         <v>58</v>
       </c>
       <c r="BY62" s="22"/>
       <c r="CA62" s="22"/>
       <c r="CC62" s="22"/>
     </row>
-    <row r="63" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
+    <row r="63" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="16">
         <v>59</v>
       </c>
       <c r="BY63" s="22"/>
       <c r="CA63" s="22"/>
       <c r="CC63" s="22"/>
     </row>
-    <row r="64" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
+    <row r="64" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="16">
         <v>60</v>
       </c>
       <c r="BY64" s="22"/>
       <c r="CA64" s="22"/>
       <c r="CC64" s="22"/>
     </row>
-    <row r="65" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
+    <row r="65" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="16">
         <v>61</v>
       </c>
       <c r="BY65" s="22"/>
       <c r="CA65" s="22"/>
       <c r="CC65" s="22"/>
     </row>
-    <row r="66" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
+    <row r="66" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="16">
         <v>62</v>
       </c>
       <c r="BY66" s="22"/>
       <c r="CA66" s="22"/>
       <c r="CC66" s="22"/>
     </row>
-    <row r="67" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
+    <row r="67" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="16">
         <v>63</v>
       </c>
       <c r="BY67" s="22"/>
       <c r="CA67" s="22"/>
       <c r="CC67" s="22"/>
     </row>
-    <row r="68" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
+    <row r="68" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="16">
         <v>64</v>
       </c>
       <c r="BY68" s="22"/>
       <c r="CA68" s="22"/>
       <c r="CC68" s="22"/>
     </row>
-    <row r="69" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
+    <row r="69" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="16">
         <v>65</v>
       </c>
       <c r="BY69" s="22"/>
       <c r="CA69" s="22"/>
       <c r="CC69" s="22"/>
     </row>
-    <row r="70" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
+    <row r="70" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="16">
         <v>66</v>
       </c>
       <c r="BY70" s="22"/>
       <c r="CA70" s="22"/>
       <c r="CC70" s="22"/>
     </row>
-    <row r="71" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
+    <row r="71" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="16">
         <v>67</v>
       </c>
       <c r="BY71" s="22"/>
       <c r="CA71" s="22"/>
       <c r="CC71" s="22"/>
     </row>
-    <row r="72" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
+    <row r="72" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="16">
         <v>68</v>
       </c>
       <c r="BY72" s="22"/>
       <c r="CA72" s="22"/>
       <c r="CC72" s="22"/>
     </row>
-    <row r="73" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
+    <row r="73" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16">
         <v>69</v>
       </c>
       <c r="BY73" s="22"/>
       <c r="CA73" s="22"/>
       <c r="CC73" s="22"/>
     </row>
-    <row r="74" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
+    <row r="74" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="16">
         <v>70</v>
       </c>
       <c r="BY74" s="22"/>
       <c r="CA74" s="22"/>
       <c r="CC74" s="22"/>
     </row>
-    <row r="75" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
+    <row r="75" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="16">
         <v>71</v>
       </c>
       <c r="BY75" s="22"/>
       <c r="CA75" s="22"/>
       <c r="CC75" s="22"/>
     </row>
-    <row r="76" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
+    <row r="76" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="16">
         <v>72</v>
       </c>
       <c r="BY76" s="22"/>
       <c r="CA76" s="22"/>
       <c r="CC76" s="22"/>
     </row>
-    <row r="77" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="17">
+    <row r="77" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="16">
         <v>73</v>
       </c>
       <c r="BY77" s="22"/>
       <c r="CA77" s="22"/>
       <c r="CC77" s="22"/>
     </row>
-    <row r="78" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17">
+    <row r="78" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="16">
         <v>74</v>
       </c>
       <c r="BY78" s="22"/>
       <c r="CA78" s="22"/>
       <c r="CC78" s="22"/>
     </row>
-    <row r="79" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="17">
+    <row r="79" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="16">
         <v>75</v>
       </c>
       <c r="BY79" s="22"/>
       <c r="CA79" s="22"/>
       <c r="CC79" s="22"/>
     </row>
-    <row r="80" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="17">
+    <row r="80" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="16">
         <v>76</v>
       </c>
       <c r="BY80" s="22"/>
       <c r="CA80" s="22"/>
       <c r="CC80" s="22"/>
     </row>
-    <row r="81" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="17">
+    <row r="81" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="16">
         <v>77</v>
       </c>
       <c r="BY81" s="22"/>
       <c r="CA81" s="22"/>
       <c r="CC81" s="22"/>
     </row>
-    <row r="82" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="17">
+    <row r="82" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="16">
         <v>78</v>
       </c>
       <c r="BY82" s="22"/>
       <c r="CA82" s="22"/>
       <c r="CC82" s="22"/>
     </row>
-    <row r="83" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="17">
+    <row r="83" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="16">
         <v>79</v>
       </c>
       <c r="BY83" s="22"/>
       <c r="CA83" s="22"/>
       <c r="CC83" s="22"/>
     </row>
-    <row r="84" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="17">
+    <row r="84" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="16">
         <v>80</v>
       </c>
       <c r="BY84" s="22"/>
       <c r="CA84" s="22"/>
       <c r="CC84" s="22"/>
     </row>
-    <row r="85" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="17">
+    <row r="85" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="16">
         <v>81</v>
       </c>
       <c r="BY85" s="22"/>
       <c r="CA85" s="22"/>
       <c r="CC85" s="22"/>
     </row>
-    <row r="86" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="17">
+    <row r="86" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="16">
         <v>82</v>
       </c>
       <c r="BY86" s="22"/>
       <c r="CA86" s="22"/>
       <c r="CC86" s="22"/>
     </row>
-    <row r="87" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="17">
+    <row r="87" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="16">
         <v>83</v>
       </c>
       <c r="BY87" s="22"/>
       <c r="CA87" s="22"/>
       <c r="CC87" s="22"/>
     </row>
-    <row r="88" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="17">
+    <row r="88" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="16">
         <v>84</v>
       </c>
       <c r="BY88" s="22"/>
       <c r="CA88" s="22"/>
       <c r="CC88" s="22"/>
     </row>
-    <row r="89" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="17">
+    <row r="89" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="16">
         <v>85</v>
       </c>
       <c r="BY89" s="22"/>
       <c r="CA89" s="22"/>
       <c r="CC89" s="22"/>
     </row>
-    <row r="90" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="17">
+    <row r="90" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="16">
         <v>86</v>
       </c>
       <c r="BY90" s="22"/>
       <c r="CA90" s="22"/>
       <c r="CC90" s="22"/>
     </row>
-    <row r="91" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="17">
+    <row r="91" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="16">
         <v>87</v>
       </c>
       <c r="BY91" s="22"/>
       <c r="CA91" s="22"/>
       <c r="CC91" s="22"/>
     </row>
-    <row r="92" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="17">
+    <row r="92" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="16">
         <v>88</v>
       </c>
       <c r="BY92" s="22"/>
       <c r="CA92" s="22"/>
       <c r="CC92" s="22"/>
     </row>
-    <row r="93" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="17">
+    <row r="93" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="16">
         <v>89</v>
       </c>
       <c r="BY93" s="22"/>
       <c r="CA93" s="22"/>
       <c r="CC93" s="22"/>
     </row>
-    <row r="94" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="17">
+    <row r="94" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="16">
         <v>90</v>
       </c>
       <c r="BY94" s="22"/>
       <c r="CA94" s="22"/>
       <c r="CC94" s="22"/>
     </row>
-    <row r="95" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="17">
+    <row r="95" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16">
         <v>91</v>
       </c>
       <c r="BY95" s="22"/>
       <c r="CA95" s="22"/>
       <c r="CC95" s="22"/>
     </row>
-    <row r="96" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="17">
+    <row r="96" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="16">
         <v>92</v>
       </c>
       <c r="BY96" s="22"/>
       <c r="CA96" s="22"/>
       <c r="CC96" s="22"/>
     </row>
-    <row r="97" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="17">
+    <row r="97" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="16">
         <v>93</v>
       </c>
       <c r="BY97" s="22"/>
       <c r="CA97" s="22"/>
       <c r="CC97" s="22"/>
     </row>
-    <row r="98" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="17">
+    <row r="98" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="16">
         <v>94</v>
       </c>
       <c r="BY98" s="22"/>
       <c r="CA98" s="22"/>
       <c r="CC98" s="22"/>
     </row>
-    <row r="99" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="17">
+    <row r="99" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="16">
         <v>95</v>
       </c>
       <c r="BY99" s="22"/>
       <c r="CA99" s="22"/>
       <c r="CC99" s="22"/>
     </row>
-    <row r="100" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="17">
+    <row r="100" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="16">
         <v>96</v>
       </c>
       <c r="BY100" s="22"/>
       <c r="CA100" s="22"/>
       <c r="CC100" s="22"/>
     </row>
-    <row r="101" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="17">
+    <row r="101" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="16">
         <v>97</v>
       </c>
       <c r="BY101" s="22"/>
       <c r="CA101" s="22"/>
       <c r="CC101" s="22"/>
     </row>
-    <row r="102" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="17">
+    <row r="102" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="16">
         <v>98</v>
       </c>
       <c r="BY102" s="22"/>
       <c r="CA102" s="22"/>
       <c r="CC102" s="22"/>
     </row>
-    <row r="103" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="17">
+    <row r="103" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="16">
         <v>99</v>
       </c>
       <c r="BY103" s="22"/>
       <c r="CA103" s="22"/>
       <c r="CC103" s="22"/>
     </row>
-    <row r="104" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="17">
+    <row r="104" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="16">
         <v>100</v>
       </c>
       <c r="BY104" s="22"/>
       <c r="CA104" s="22"/>
       <c r="CC104" s="22"/>
     </row>
-    <row r="105" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="17">
+    <row r="105" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="16">
         <v>101</v>
       </c>
       <c r="BY105" s="22"/>
       <c r="CA105" s="22"/>
       <c r="CC105" s="22"/>
     </row>
-    <row r="106" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="17">
+    <row r="106" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="16">
         <v>102</v>
       </c>
       <c r="BY106" s="22"/>
       <c r="CA106" s="22"/>
       <c r="CC106" s="22"/>
     </row>
-    <row r="107" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="17">
+    <row r="107" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="16">
         <v>103</v>
       </c>
       <c r="BY107" s="22"/>
       <c r="CA107" s="22"/>
       <c r="CC107" s="22"/>
     </row>
-    <row r="108" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="17">
+    <row r="108" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="16">
         <v>104</v>
       </c>
       <c r="BY108" s="22"/>
       <c r="CA108" s="22"/>
       <c r="CC108" s="22"/>
     </row>
-    <row r="109" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="17">
+    <row r="109" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="16">
         <v>105</v>
       </c>
       <c r="BY109" s="22"/>
       <c r="CA109" s="22"/>
       <c r="CC109" s="22"/>
     </row>
-    <row r="110" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="17">
+    <row r="110" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="16">
         <v>106</v>
       </c>
       <c r="BY110" s="22"/>
       <c r="CA110" s="22"/>
       <c r="CC110" s="22"/>
     </row>
-    <row r="111" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="17">
+    <row r="111" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="16">
         <v>107</v>
       </c>
       <c r="BY111" s="22"/>
       <c r="CA111" s="22"/>
       <c r="CC111" s="22"/>
     </row>
-    <row r="112" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="17">
+    <row r="112" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="16">
         <v>108</v>
       </c>
       <c r="BY112" s="22"/>
       <c r="CA112" s="22"/>
       <c r="CC112" s="22"/>
     </row>
-    <row r="113" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="17">
+    <row r="113" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="16">
         <v>109</v>
       </c>
       <c r="BY113" s="22"/>
       <c r="CA113" s="22"/>
       <c r="CC113" s="22"/>
     </row>
-    <row r="114" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="17">
+    <row r="114" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="16">
         <v>110</v>
       </c>
       <c r="BY114" s="22"/>
       <c r="CA114" s="22"/>
       <c r="CC114" s="22"/>
     </row>
-    <row r="115" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="17">
+    <row r="115" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="16">
         <v>111</v>
       </c>
       <c r="BY115" s="22"/>
       <c r="CA115" s="22"/>
       <c r="CC115" s="22"/>
     </row>
-    <row r="116" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="17">
+    <row r="116" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="16">
         <v>112</v>
       </c>
       <c r="BY116" s="22"/>
       <c r="CA116" s="22"/>
       <c r="CC116" s="22"/>
     </row>
-    <row r="117" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="17">
+    <row r="117" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="16">
         <v>113</v>
       </c>
       <c r="BY117" s="22"/>
       <c r="CA117" s="22"/>
       <c r="CC117" s="22"/>
     </row>
-    <row r="118" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="17">
+    <row r="118" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="16">
         <v>114</v>
       </c>
       <c r="BY118" s="22"/>
       <c r="CA118" s="22"/>
       <c r="CC118" s="22"/>
     </row>
-    <row r="119" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="17">
+    <row r="119" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="16">
         <v>115</v>
       </c>
       <c r="BY119" s="22"/>
       <c r="CA119" s="22"/>
       <c r="CC119" s="22"/>
     </row>
-    <row r="120" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="17">
+    <row r="120" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="16">
         <v>116</v>
       </c>
       <c r="BY120" s="22"/>
       <c r="CA120" s="22"/>
       <c r="CC120" s="22"/>
     </row>
-    <row r="121" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="17">
+    <row r="121" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="16">
         <v>117</v>
       </c>
       <c r="BY121" s="22"/>
       <c r="CA121" s="22"/>
       <c r="CC121" s="22"/>
     </row>
-    <row r="122" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="17">
+    <row r="122" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="16">
         <v>118</v>
       </c>
       <c r="BY122" s="22"/>
       <c r="CA122" s="22"/>
       <c r="CC122" s="22"/>
     </row>
-    <row r="123" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="17">
+    <row r="123" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="16">
         <v>119</v>
       </c>
       <c r="BY123" s="22"/>
       <c r="CA123" s="22"/>
       <c r="CC123" s="22"/>
     </row>
-    <row r="124" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="17">
+    <row r="124" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="16">
         <v>120</v>
       </c>
       <c r="BY124" s="22"/>
       <c r="CA124" s="22"/>
       <c r="CC124" s="22"/>
     </row>
-    <row r="125" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="17">
+    <row r="125" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="16">
         <v>121</v>
       </c>
       <c r="BY125" s="22"/>
       <c r="CA125" s="22"/>
       <c r="CC125" s="22"/>
     </row>
-    <row r="126" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="17">
+    <row r="126" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="16">
         <v>122</v>
       </c>
       <c r="BY126" s="22"/>
       <c r="CA126" s="22"/>
       <c r="CC126" s="22"/>
     </row>
-    <row r="127" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="17">
+    <row r="127" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="16">
         <v>123</v>
       </c>
       <c r="BY127" s="22"/>
       <c r="CA127" s="22"/>
       <c r="CC127" s="22"/>
     </row>
-    <row r="128" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="17">
+    <row r="128" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="16">
         <v>124</v>
       </c>
       <c r="BY128" s="22"/>
       <c r="CA128" s="22"/>
       <c r="CC128" s="22"/>
     </row>
-    <row r="129" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="17">
+    <row r="129" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="16">
         <v>125</v>
       </c>
       <c r="BY129" s="22"/>
       <c r="CA129" s="22"/>
       <c r="CC129" s="22"/>
     </row>
-    <row r="130" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="17">
+    <row r="130" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="16">
         <v>126</v>
       </c>
       <c r="BY130" s="22"/>
       <c r="CA130" s="22"/>
       <c r="CC130" s="22"/>
     </row>
-    <row r="131" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="17">
+    <row r="131" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="16">
         <v>127</v>
       </c>
       <c r="BY131" s="22"/>
       <c r="CA131" s="22"/>
       <c r="CC131" s="22"/>
     </row>
-    <row r="132" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="17">
+    <row r="132" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="16">
         <v>128</v>
       </c>
       <c r="BY132" s="22"/>
       <c r="CA132" s="22"/>
       <c r="CC132" s="22"/>
     </row>
-    <row r="133" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="17">
+    <row r="133" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="16">
         <v>129</v>
       </c>
       <c r="BY133" s="22"/>
       <c r="CA133" s="22"/>
       <c r="CC133" s="22"/>
     </row>
-    <row r="134" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="17">
+    <row r="134" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="16">
         <v>130</v>
       </c>
       <c r="BY134" s="22"/>
       <c r="CA134" s="22"/>
       <c r="CC134" s="22"/>
     </row>
-    <row r="135" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="17">
+    <row r="135" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="16">
         <v>131</v>
       </c>
       <c r="BY135" s="22"/>
       <c r="CA135" s="22"/>
       <c r="CC135" s="22"/>
     </row>
-    <row r="136" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="17">
+    <row r="136" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="16">
         <v>132</v>
       </c>
       <c r="BY136" s="22"/>
       <c r="CA136" s="22"/>
       <c r="CC136" s="22"/>
     </row>
-    <row r="137" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="17">
+    <row r="137" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="16">
         <v>133</v>
       </c>
       <c r="BY137" s="22"/>
       <c r="CA137" s="22"/>
       <c r="CC137" s="22"/>
     </row>
-    <row r="138" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="17">
+    <row r="138" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="16">
         <v>134</v>
       </c>
       <c r="BY138" s="22"/>
       <c r="CA138" s="22"/>
       <c r="CC138" s="22"/>
     </row>
-    <row r="139" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="17">
+    <row r="139" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="16">
         <v>135</v>
       </c>
       <c r="BY139" s="22"/>
       <c r="CA139" s="22"/>
       <c r="CC139" s="22"/>
     </row>
-    <row r="140" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="17">
+    <row r="140" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="16">
         <v>136</v>
       </c>
       <c r="BY140" s="22"/>
       <c r="CA140" s="22"/>
       <c r="CC140" s="22"/>
     </row>
-    <row r="141" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="17">
+    <row r="141" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="16">
         <v>137</v>
       </c>
       <c r="BY141" s="22"/>
       <c r="CA141" s="22"/>
       <c r="CC141" s="22"/>
     </row>
-    <row r="142" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="17">
+    <row r="142" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="16">
         <v>138</v>
       </c>
       <c r="BY142" s="22"/>
       <c r="CA142" s="22"/>
       <c r="CC142" s="22"/>
     </row>
-    <row r="143" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="17">
+    <row r="143" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="16">
         <v>139</v>
       </c>
       <c r="BY143" s="22"/>
       <c r="CA143" s="22"/>
       <c r="CC143" s="22"/>
     </row>
-    <row r="144" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="17">
+    <row r="144" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="16">
         <v>140</v>
       </c>
       <c r="BY144" s="22"/>
       <c r="CA144" s="22"/>
       <c r="CC144" s="22"/>
     </row>
-    <row r="145" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="17">
+    <row r="145" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="16">
         <v>141</v>
       </c>
       <c r="BY145" s="22"/>
       <c r="CA145" s="22"/>
       <c r="CC145" s="22"/>
     </row>
-    <row r="146" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="17">
+    <row r="146" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="16">
         <v>142</v>
       </c>
       <c r="BY146" s="22"/>
       <c r="CA146" s="22"/>
       <c r="CC146" s="22"/>
     </row>
-    <row r="147" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="17">
+    <row r="147" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="16">
         <v>143</v>
       </c>
       <c r="BY147" s="22"/>
       <c r="CA147" s="22"/>
       <c r="CC147" s="22"/>
     </row>
-    <row r="148" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="17">
+    <row r="148" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="16">
         <v>144</v>
       </c>
       <c r="BY148" s="22"/>
       <c r="CA148" s="22"/>
       <c r="CC148" s="22"/>
     </row>
-    <row r="149" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="17">
+    <row r="149" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A149" s="16">
         <v>145</v>
       </c>
       <c r="BY149" s="22"/>
       <c r="CA149" s="22"/>
       <c r="CC149" s="22"/>
     </row>
-    <row r="150" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="17">
+    <row r="150" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="16">
         <v>146</v>
       </c>
       <c r="BY150" s="22"/>
       <c r="CA150" s="22"/>
       <c r="CC150" s="22"/>
     </row>
-    <row r="151" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="17">
+    <row r="151" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="16">
         <v>147</v>
       </c>
       <c r="BY151" s="22"/>
       <c r="CA151" s="22"/>
       <c r="CC151" s="22"/>
     </row>
-    <row r="152" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="17">
+    <row r="152" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="16">
         <v>148</v>
       </c>
       <c r="BY152" s="22"/>
       <c r="CA152" s="22"/>
       <c r="CC152" s="22"/>
     </row>
-    <row r="153" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="17">
+    <row r="153" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="16">
         <v>149</v>
       </c>
       <c r="BY153" s="22"/>
       <c r="CA153" s="22"/>
       <c r="CC153" s="22"/>
     </row>
-    <row r="154" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="17">
+    <row r="154" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="16">
         <v>150</v>
       </c>
       <c r="BY154" s="22"/>
       <c r="CA154" s="22"/>
       <c r="CC154" s="22"/>
     </row>
-    <row r="155" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="17">
+    <row r="155" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="16">
         <v>151</v>
       </c>
       <c r="BY155" s="22"/>
       <c r="CA155" s="22"/>
       <c r="CC155" s="22"/>
     </row>
-    <row r="156" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="17">
+    <row r="156" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="16">
         <v>152</v>
       </c>
       <c r="BY156" s="22"/>
       <c r="CA156" s="22"/>
       <c r="CC156" s="22"/>
     </row>
-    <row r="157" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="17">
+    <row r="157" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="16">
         <v>153</v>
       </c>
       <c r="BY157" s="22"/>
       <c r="CA157" s="22"/>
       <c r="CC157" s="22"/>
     </row>
-    <row r="158" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="17">
+    <row r="158" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="16">
         <v>154</v>
       </c>
       <c r="BY158" s="22"/>
       <c r="CA158" s="22"/>
       <c r="CC158" s="22"/>
     </row>
-    <row r="159" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="17">
+    <row r="159" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="16">
         <v>155</v>
       </c>
       <c r="BY159" s="22"/>
       <c r="CA159" s="22"/>
       <c r="CC159" s="22"/>
     </row>
-    <row r="160" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="17">
+    <row r="160" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="16">
         <v>156</v>
       </c>
       <c r="BY160" s="22"/>
       <c r="CA160" s="22"/>
       <c r="CC160" s="22"/>
     </row>
-    <row r="161" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="17">
+    <row r="161" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="16">
         <v>157</v>
       </c>
       <c r="BY161" s="22"/>
       <c r="CA161" s="22"/>
       <c r="CC161" s="22"/>
     </row>
-    <row r="162" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="17">
+    <row r="162" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="16">
         <v>158</v>
       </c>
       <c r="BY162" s="22"/>
       <c r="CA162" s="22"/>
       <c r="CC162" s="22"/>
     </row>
-    <row r="163" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="17">
+    <row r="163" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="16">
         <v>159</v>
       </c>
       <c r="BY163" s="22"/>
       <c r="CA163" s="22"/>
       <c r="CC163" s="22"/>
     </row>
-    <row r="164" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="17">
+    <row r="164" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="16">
         <v>160</v>
       </c>
       <c r="BY164" s="22"/>
       <c r="CA164" s="22"/>
       <c r="CC164" s="22"/>
     </row>
-    <row r="165" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="17">
+    <row r="165" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="16">
         <v>161</v>
       </c>
       <c r="BY165" s="22"/>
       <c r="CA165" s="22"/>
       <c r="CC165" s="22"/>
     </row>
-    <row r="166" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="17">
+    <row r="166" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="16">
         <v>162</v>
       </c>
       <c r="BY166" s="22"/>
       <c r="CA166" s="22"/>
       <c r="CC166" s="22"/>
     </row>
-    <row r="167" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="17">
+    <row r="167" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="16">
         <v>163</v>
       </c>
       <c r="BY167" s="22"/>
       <c r="CA167" s="22"/>
       <c r="CC167" s="22"/>
     </row>
-    <row r="168" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A168" s="17">
+    <row r="168" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="16">
         <v>164</v>
       </c>
       <c r="BY168" s="22"/>
       <c r="CA168" s="22"/>
       <c r="CC168" s="22"/>
     </row>
-    <row r="169" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A169" s="17">
+    <row r="169" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="16">
         <v>165</v>
       </c>
       <c r="BY169" s="22"/>
       <c r="CA169" s="22"/>
       <c r="CC169" s="22"/>
     </row>
-    <row r="170" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A170" s="17">
+    <row r="170" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="16">
         <v>166</v>
       </c>
       <c r="BY170" s="22"/>
       <c r="CA170" s="22"/>
       <c r="CC170" s="22"/>
     </row>
-    <row r="171" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="17">
+    <row r="171" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="16">
         <v>167</v>
       </c>
       <c r="BY171" s="22"/>
       <c r="CA171" s="22"/>
       <c r="CC171" s="22"/>
     </row>
-    <row r="172" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="17">
+    <row r="172" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="16">
         <v>168</v>
       </c>
       <c r="BY172" s="22"/>
       <c r="CA172" s="22"/>
       <c r="CC172" s="22"/>
     </row>
-    <row r="173" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="17">
+    <row r="173" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="16">
         <v>169</v>
       </c>
       <c r="BY173" s="22"/>
       <c r="CA173" s="22"/>
       <c r="CC173" s="22"/>
     </row>
-    <row r="174" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="17">
+    <row r="174" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="16">
         <v>170</v>
       </c>
       <c r="BY174" s="22"/>
       <c r="CA174" s="22"/>
       <c r="CC174" s="22"/>
     </row>
-    <row r="175" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="17">
+    <row r="175" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="16">
         <v>171</v>
       </c>
       <c r="BY175" s="22"/>
       <c r="CA175" s="22"/>
       <c r="CC175" s="22"/>
     </row>
-    <row r="176" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="17">
+    <row r="176" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="16">
         <v>172</v>
       </c>
       <c r="BY176" s="22"/>
       <c r="CA176" s="22"/>
       <c r="CC176" s="22"/>
     </row>
-    <row r="177" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A177" s="17">
+    <row r="177" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="16">
         <v>173</v>
       </c>
       <c r="BY177" s="22"/>
       <c r="CA177" s="22"/>
       <c r="CC177" s="22"/>
     </row>
-    <row r="178" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A178" s="17">
+    <row r="178" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="16">
         <v>174</v>
       </c>
       <c r="BY178" s="22"/>
       <c r="CA178" s="22"/>
       <c r="CC178" s="22"/>
     </row>
-    <row r="179" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A179" s="17">
+    <row r="179" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="16">
         <v>175</v>
       </c>
       <c r="BY179" s="22"/>
       <c r="CA179" s="22"/>
       <c r="CC179" s="22"/>
     </row>
-    <row r="180" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A180" s="17">
+    <row r="180" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="16">
         <v>176</v>
       </c>
       <c r="BY180" s="22"/>
       <c r="CA180" s="22"/>
       <c r="CC180" s="22"/>
     </row>
-    <row r="181" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A181" s="17">
+    <row r="181" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="16">
         <v>177</v>
       </c>
       <c r="BY181" s="22"/>
       <c r="CA181" s="22"/>
       <c r="CC181" s="22"/>
     </row>
-    <row r="182" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A182" s="17">
+    <row r="182" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="16">
         <v>178</v>
       </c>
       <c r="BY182" s="22"/>
       <c r="CA182" s="22"/>
       <c r="CC182" s="22"/>
     </row>
-    <row r="183" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A183" s="17">
+    <row r="183" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="16">
         <v>179</v>
       </c>
       <c r="BY183" s="22"/>
       <c r="CA183" s="22"/>
       <c r="CC183" s="22"/>
     </row>
-    <row r="184" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A184" s="17">
+    <row r="184" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="16">
         <v>180</v>
       </c>
       <c r="BY184" s="22"/>
       <c r="CA184" s="22"/>
       <c r="CC184" s="22"/>
     </row>
-    <row r="185" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A185" s="17">
+    <row r="185" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="16">
         <v>181</v>
       </c>
       <c r="BY185" s="22"/>
       <c r="CA185" s="22"/>
       <c r="CC185" s="22"/>
     </row>
-    <row r="186" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="17">
+    <row r="186" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="16">
         <v>182</v>
       </c>
       <c r="BY186" s="22"/>
       <c r="CA186" s="22"/>
       <c r="CC186" s="22"/>
     </row>
-    <row r="187" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="17">
+    <row r="187" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="16">
         <v>183</v>
       </c>
       <c r="BY187" s="22"/>
       <c r="CA187" s="22"/>
       <c r="CC187" s="22"/>
     </row>
-    <row r="188" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A188" s="17">
+    <row r="188" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="16">
         <v>184</v>
       </c>
       <c r="BY188" s="22"/>
       <c r="CA188" s="22"/>
       <c r="CC188" s="22"/>
     </row>
-    <row r="189" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A189" s="17">
+    <row r="189" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="16">
         <v>185</v>
       </c>
       <c r="BY189" s="22"/>
       <c r="CA189" s="22"/>
       <c r="CC189" s="22"/>
     </row>
-    <row r="190" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="17">
+    <row r="190" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="16">
         <v>186</v>
       </c>
       <c r="BY190" s="22"/>
       <c r="CA190" s="22"/>
       <c r="CC190" s="22"/>
     </row>
-    <row r="191" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="17">
+    <row r="191" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="16">
         <v>187</v>
       </c>
       <c r="BY191" s="22"/>
       <c r="CA191" s="22"/>
       <c r="CC191" s="22"/>
     </row>
-    <row r="192" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="17">
+    <row r="192" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="16">
         <v>188</v>
       </c>
       <c r="BY192" s="22"/>
       <c r="CA192" s="22"/>
       <c r="CC192" s="22"/>
     </row>
-    <row r="193" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="17">
+    <row r="193" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="16">
         <v>189</v>
       </c>
       <c r="BY193" s="22"/>
       <c r="CA193" s="22"/>
       <c r="CC193" s="22"/>
     </row>
-    <row r="194" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="17">
+    <row r="194" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="16">
         <v>190</v>
       </c>
       <c r="BY194" s="22"/>
       <c r="CA194" s="22"/>
       <c r="CC194" s="22"/>
     </row>
-    <row r="195" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="17">
+    <row r="195" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="16">
         <v>191</v>
       </c>
       <c r="BY195" s="22"/>
       <c r="CA195" s="22"/>
       <c r="CC195" s="22"/>
     </row>
-    <row r="196" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A196" s="17">
+    <row r="196" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="16">
         <v>192</v>
       </c>
       <c r="BY196" s="22"/>
       <c r="CA196" s="22"/>
       <c r="CC196" s="22"/>
     </row>
-    <row r="197" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A197" s="17">
+    <row r="197" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="16">
         <v>193</v>
       </c>
       <c r="BY197" s="22"/>
       <c r="CA197" s="22"/>
       <c r="CC197" s="22"/>
     </row>
-    <row r="198" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A198" s="17">
+    <row r="198" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="16">
         <v>194</v>
       </c>
       <c r="BY198" s="22"/>
       <c r="CA198" s="22"/>
       <c r="CC198" s="22"/>
     </row>
-    <row r="199" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A199" s="17">
+    <row r="199" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="16">
         <v>195</v>
       </c>
       <c r="BY199" s="22"/>
       <c r="CA199" s="22"/>
       <c r="CC199" s="22"/>
     </row>
-    <row r="200" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="17">
+    <row r="200" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="16">
         <v>196</v>
       </c>
       <c r="BY200" s="22"/>
       <c r="CA200" s="22"/>
       <c r="CC200" s="22"/>
     </row>
-    <row r="201" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="17">
+    <row r="201" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="16">
         <v>197</v>
       </c>
       <c r="BY201" s="22"/>
       <c r="CA201" s="22"/>
       <c r="CC201" s="22"/>
     </row>
-    <row r="202" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="17">
+    <row r="202" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="16">
         <v>198</v>
       </c>
       <c r="BY202" s="22"/>
       <c r="CA202" s="22"/>
       <c r="CC202" s="22"/>
     </row>
-    <row r="203" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="17">
+    <row r="203" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="16">
         <v>199</v>
       </c>
       <c r="BY203" s="22"/>
       <c r="CA203" s="22"/>
       <c r="CC203" s="22"/>
     </row>
-    <row r="204" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="17">
+    <row r="204" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="16">
         <v>200</v>
       </c>
       <c r="BY204" s="22"/>
       <c r="CA204" s="22"/>
       <c r="CC204" s="22"/>
     </row>
-    <row r="205" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="17">
+    <row r="205" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="16">
         <v>201</v>
       </c>
       <c r="BY205" s="22"/>
       <c r="CA205" s="22"/>
       <c r="CC205" s="22"/>
     </row>
-    <row r="206" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="17">
+    <row r="206" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="16">
         <v>202</v>
       </c>
       <c r="BY206" s="22"/>
       <c r="CA206" s="22"/>
       <c r="CC206" s="22"/>
     </row>
-    <row r="207" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="17">
+    <row r="207" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="16">
         <v>203</v>
       </c>
       <c r="BY207" s="22"/>
       <c r="CA207" s="22"/>
       <c r="CC207" s="22"/>
     </row>
-    <row r="208" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="17">
+    <row r="208" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="16">
         <v>204</v>
       </c>
       <c r="BY208" s="22"/>
       <c r="CA208" s="22"/>
       <c r="CC208" s="22"/>
     </row>
-    <row r="209" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="17">
+    <row r="209" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="16">
         <v>205</v>
       </c>
       <c r="BY209" s="22"/>
       <c r="CA209" s="22"/>
       <c r="CC209" s="22"/>
     </row>
-    <row r="210" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="17">
+    <row r="210" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="16">
         <v>206</v>
       </c>
       <c r="BY210" s="22"/>
       <c r="CA210" s="22"/>
       <c r="CC210" s="22"/>
     </row>
-    <row r="211" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="17">
+    <row r="211" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="16">
         <v>207</v>
       </c>
       <c r="BY211" s="22"/>
       <c r="CA211" s="22"/>
       <c r="CC211" s="22"/>
     </row>
-    <row r="212" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="17">
+    <row r="212" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="16">
         <v>208</v>
       </c>
       <c r="BY212" s="22"/>
       <c r="CA212" s="22"/>
       <c r="CC212" s="22"/>
     </row>
-    <row r="213" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="17">
+    <row r="213" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="16">
         <v>209</v>
       </c>
       <c r="BY213" s="22"/>
       <c r="CA213" s="22"/>
       <c r="CC213" s="22"/>
     </row>
-    <row r="214" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="17">
+    <row r="214" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="16">
         <v>210</v>
       </c>
       <c r="BY214" s="22"/>
       <c r="CA214" s="22"/>
       <c r="CC214" s="22"/>
     </row>
-    <row r="215" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="17">
+    <row r="215" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="16">
         <v>211</v>
       </c>
       <c r="BY215" s="22"/>
       <c r="CA215" s="22"/>
       <c r="CC215" s="22"/>
     </row>
-    <row r="216" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="17">
+    <row r="216" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="16">
         <v>212</v>
       </c>
       <c r="BY216" s="22"/>
       <c r="CA216" s="22"/>
       <c r="CC216" s="22"/>
     </row>
-    <row r="217" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="17">
+    <row r="217" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="16">
         <v>213</v>
       </c>
       <c r="BY217" s="22"/>
       <c r="CA217" s="22"/>
       <c r="CC217" s="22"/>
     </row>
-    <row r="218" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="17">
+    <row r="218" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="16">
         <v>214</v>
       </c>
       <c r="BY218" s="22"/>
       <c r="CA218" s="22"/>
       <c r="CC218" s="22"/>
     </row>
-    <row r="219" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="17">
+    <row r="219" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="16">
         <v>215</v>
       </c>
       <c r="BY219" s="22"/>
       <c r="CA219" s="22"/>
       <c r="CC219" s="22"/>
     </row>
-    <row r="220" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="17">
+    <row r="220" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="16">
         <v>216</v>
       </c>
       <c r="BY220" s="22"/>
       <c r="CA220" s="22"/>
       <c r="CC220" s="22"/>
     </row>
-    <row r="221" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="17">
+    <row r="221" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="16">
         <v>217</v>
       </c>
       <c r="BY221" s="22"/>
       <c r="CA221" s="22"/>
       <c r="CC221" s="22"/>
     </row>
-    <row r="222" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="17">
+    <row r="222" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="16">
         <v>218</v>
       </c>
       <c r="BY222" s="22"/>
       <c r="CA222" s="22"/>
       <c r="CC222" s="22"/>
     </row>
-    <row r="223" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="17">
+    <row r="223" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="16">
         <v>219</v>
       </c>
       <c r="BY223" s="22"/>
       <c r="CA223" s="22"/>
       <c r="CC223" s="22"/>
     </row>
-    <row r="224" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="17">
+    <row r="224" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="16">
         <v>220</v>
       </c>
       <c r="BY224" s="22"/>
       <c r="CA224" s="22"/>
       <c r="CC224" s="22"/>
     </row>
-    <row r="225" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="17">
+    <row r="225" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="16">
         <v>221</v>
       </c>
       <c r="BY225" s="22"/>
       <c r="CA225" s="22"/>
       <c r="CC225" s="22"/>
     </row>
-    <row r="226" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="17">
+    <row r="226" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="16">
         <v>222</v>
       </c>
       <c r="BY226" s="22"/>
       <c r="CA226" s="22"/>
       <c r="CC226" s="22"/>
     </row>
-    <row r="227" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="17">
+    <row r="227" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="16">
         <v>223</v>
       </c>
       <c r="BY227" s="22"/>
       <c r="CA227" s="22"/>
       <c r="CC227" s="22"/>
     </row>
-    <row r="228" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="17">
+    <row r="228" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A228" s="16">
         <v>224</v>
       </c>
       <c r="BY228" s="22"/>
       <c r="CA228" s="22"/>
       <c r="CC228" s="22"/>
     </row>
-    <row r="229" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="17">
+    <row r="229" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="16">
         <v>225</v>
       </c>
       <c r="BY229" s="22"/>
       <c r="CA229" s="22"/>
       <c r="CC229" s="22"/>
     </row>
-    <row r="230" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="17">
+    <row r="230" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="16">
         <v>226</v>
       </c>
       <c r="BY230" s="22"/>
       <c r="CA230" s="22"/>
       <c r="CC230" s="22"/>
     </row>
-    <row r="231" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="17">
+    <row r="231" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="16">
         <v>227</v>
       </c>
       <c r="BY231" s="22"/>
       <c r="CA231" s="22"/>
       <c r="CC231" s="22"/>
     </row>
-    <row r="232" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="17">
+    <row r="232" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="16">
         <v>228</v>
       </c>
       <c r="BY232" s="22"/>
       <c r="CA232" s="22"/>
       <c r="CC232" s="22"/>
     </row>
-    <row r="233" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="17">
+    <row r="233" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="16">
         <v>229</v>
       </c>
       <c r="BY233" s="22"/>
       <c r="CA233" s="22"/>
       <c r="CC233" s="22"/>
     </row>
-    <row r="234" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="17">
+    <row r="234" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="16">
         <v>230</v>
       </c>
       <c r="BY234" s="22"/>
       <c r="CA234" s="22"/>
       <c r="CC234" s="22"/>
     </row>
-    <row r="235" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="17">
+    <row r="235" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="16">
         <v>231</v>
       </c>
       <c r="BY235" s="22"/>
       <c r="CA235" s="22"/>
       <c r="CC235" s="22"/>
     </row>
-    <row r="236" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="17">
+    <row r="236" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="16">
         <v>232</v>
       </c>
       <c r="BY236" s="22"/>
       <c r="CA236" s="22"/>
       <c r="CC236" s="22"/>
     </row>
-    <row r="237" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="17">
+    <row r="237" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="16">
         <v>233</v>
       </c>
       <c r="BY237" s="22"/>
       <c r="CA237" s="22"/>
       <c r="CC237" s="22"/>
     </row>
-    <row r="238" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="17">
+    <row r="238" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="16">
         <v>234</v>
       </c>
       <c r="BY238" s="22"/>
       <c r="CA238" s="22"/>
       <c r="CC238" s="22"/>
     </row>
-    <row r="239" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="17">
+    <row r="239" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="16">
         <v>235</v>
       </c>
       <c r="BY239" s="22"/>
       <c r="CA239" s="22"/>
       <c r="CC239" s="22"/>
     </row>
-    <row r="240" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="17">
+    <row r="240" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="16">
         <v>236</v>
       </c>
       <c r="BY240" s="22"/>
       <c r="CA240" s="22"/>
       <c r="CC240" s="22"/>
     </row>
-    <row r="241" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="17">
+    <row r="241" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="16">
         <v>237</v>
       </c>
       <c r="BY241" s="22"/>
       <c r="CA241" s="22"/>
       <c r="CC241" s="22"/>
     </row>
-    <row r="242" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="17">
+    <row r="242" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="16">
         <v>238</v>
       </c>
       <c r="BY242" s="22"/>
       <c r="CA242" s="22"/>
       <c r="CC242" s="22"/>
     </row>
-    <row r="243" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="17">
+    <row r="243" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="16">
         <v>239</v>
       </c>
       <c r="BY243" s="22"/>
       <c r="CA243" s="22"/>
       <c r="CC243" s="22"/>
     </row>
-    <row r="244" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="17">
+    <row r="244" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="16">
         <v>240</v>
       </c>
       <c r="BY244" s="22"/>
       <c r="CA244" s="22"/>
       <c r="CC244" s="22"/>
     </row>
-    <row r="245" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="17">
+    <row r="245" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="16">
         <v>241</v>
       </c>
       <c r="BY245" s="22"/>
       <c r="CA245" s="22"/>
       <c r="CC245" s="22"/>
     </row>
-    <row r="246" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="17">
+    <row r="246" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="16">
         <v>242</v>
       </c>
       <c r="BY246" s="22"/>
       <c r="CA246" s="22"/>
       <c r="CC246" s="22"/>
     </row>
-    <row r="247" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A247" s="17">
+    <row r="247" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="16">
         <v>243</v>
       </c>
       <c r="BY247" s="22"/>
       <c r="CA247" s="22"/>
       <c r="CC247" s="22"/>
     </row>
-    <row r="248" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="17">
+    <row r="248" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A248" s="16">
         <v>244</v>
       </c>
       <c r="BY248" s="22"/>
       <c r="CA248" s="22"/>
       <c r="CC248" s="22"/>
     </row>
-    <row r="249" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="17">
+    <row r="249" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="16">
         <v>245</v>
       </c>
       <c r="BY249" s="22"/>
       <c r="CA249" s="22"/>
       <c r="CC249" s="22"/>
     </row>
-    <row r="250" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="17">
+    <row r="250" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="16">
         <v>246</v>
       </c>
       <c r="BY250" s="22"/>
       <c r="CA250" s="22"/>
       <c r="CC250" s="22"/>
     </row>
-    <row r="251" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="17">
+    <row r="251" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="16">
         <v>247</v>
       </c>
       <c r="BY251" s="22"/>
       <c r="CA251" s="22"/>
       <c r="CC251" s="22"/>
     </row>
-    <row r="252" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="17">
+    <row r="252" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="16">
         <v>248</v>
       </c>
       <c r="BY252" s="22"/>
       <c r="CA252" s="22"/>
       <c r="CC252" s="22"/>
     </row>
-    <row r="253" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="17">
+    <row r="253" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="16">
         <v>249</v>
       </c>
       <c r="BY253" s="22"/>
       <c r="CA253" s="22"/>
       <c r="CC253" s="22"/>
     </row>
-    <row r="254" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="17">
+    <row r="254" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="16">
         <v>250</v>
       </c>
       <c r="BY254" s="22"/>
       <c r="CA254" s="22"/>
       <c r="CC254" s="22"/>
     </row>
-    <row r="255" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A255" s="17">
+    <row r="255" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="16">
         <v>251</v>
       </c>
       <c r="BY255" s="22"/>
       <c r="CA255" s="22"/>
       <c r="CC255" s="22"/>
     </row>
-    <row r="256" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A256" s="17">
+    <row r="256" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="16">
         <v>252</v>
       </c>
       <c r="BY256" s="22"/>
       <c r="CA256" s="22"/>
       <c r="CC256" s="22"/>
     </row>
-    <row r="257" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A257" s="17">
+    <row r="257" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="16">
         <v>253</v>
       </c>
       <c r="BY257" s="22"/>
       <c r="CA257" s="22"/>
       <c r="CC257" s="22"/>
     </row>
-    <row r="258" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A258" s="17">
+    <row r="258" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="16">
         <v>254</v>
       </c>
       <c r="BY258" s="22"/>
       <c r="CA258" s="22"/>
       <c r="CC258" s="22"/>
     </row>
-    <row r="259" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A259" s="17">
+    <row r="259" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="16">
         <v>255</v>
       </c>
       <c r="BY259" s="22"/>
       <c r="CA259" s="22"/>
       <c r="CC259" s="22"/>
     </row>
-    <row r="260" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A260" s="17">
+    <row r="260" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="16">
         <v>256</v>
       </c>
       <c r="BY260" s="22"/>
       <c r="CA260" s="22"/>
       <c r="CC260" s="22"/>
     </row>
-    <row r="261" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="17">
+    <row r="261" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="16">
         <v>257</v>
       </c>
       <c r="BY261" s="22"/>
       <c r="CA261" s="22"/>
       <c r="CC261" s="22"/>
     </row>
-    <row r="262" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A262" s="17">
+    <row r="262" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="16">
         <v>258</v>
       </c>
       <c r="BY262" s="22"/>
       <c r="CA262" s="22"/>
       <c r="CC262" s="22"/>
     </row>
-    <row r="263" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="17">
+    <row r="263" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="16">
         <v>259</v>
       </c>
       <c r="BY263" s="22"/>
       <c r="CA263" s="22"/>
       <c r="CC263" s="22"/>
     </row>
-    <row r="264" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A264" s="17">
+    <row r="264" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="16">
         <v>260</v>
       </c>
       <c r="BY264" s="22"/>
       <c r="CA264" s="22"/>
       <c r="CC264" s="22"/>
     </row>
-    <row r="265" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A265" s="17">
+    <row r="265" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="16">
         <v>261</v>
       </c>
       <c r="BY265" s="22"/>
       <c r="CA265" s="22"/>
       <c r="CC265" s="22"/>
     </row>
-    <row r="266" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A266" s="17">
+    <row r="266" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="16">
         <v>262</v>
       </c>
       <c r="BY266" s="22"/>
       <c r="CA266" s="22"/>
       <c r="CC266" s="22"/>
     </row>
-    <row r="267" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A267" s="17">
+    <row r="267" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="16">
         <v>263</v>
       </c>
       <c r="BY267" s="22"/>
       <c r="CA267" s="22"/>
       <c r="CC267" s="22"/>
     </row>
-    <row r="268" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A268" s="17">
+    <row r="268" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="16">
         <v>264</v>
       </c>
       <c r="BY268" s="22"/>
       <c r="CA268" s="22"/>
       <c r="CC268" s="22"/>
     </row>
-    <row r="269" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A269" s="17">
+    <row r="269" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="16">
         <v>265</v>
       </c>
       <c r="BY269" s="22"/>
       <c r="CA269" s="22"/>
       <c r="CC269" s="22"/>
     </row>
-    <row r="270" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A270" s="17">
+    <row r="270" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A270" s="16">
         <v>266</v>
       </c>
       <c r="BY270" s="22"/>
       <c r="CA270" s="22"/>
       <c r="CC270" s="22"/>
     </row>
-    <row r="271" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A271" s="17">
+    <row r="271" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A271" s="16">
         <v>267</v>
       </c>
       <c r="BY271" s="22"/>
       <c r="CA271" s="22"/>
       <c r="CC271" s="22"/>
     </row>
-    <row r="272" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A272" s="17">
+    <row r="272" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A272" s="16">
         <v>268</v>
       </c>
       <c r="BY272" s="22"/>
       <c r="CA272" s="22"/>
       <c r="CC272" s="22"/>
     </row>
-    <row r="273" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A273" s="17">
+    <row r="273" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A273" s="16">
         <v>269</v>
       </c>
       <c r="BY273" s="22"/>
       <c r="CA273" s="22"/>
       <c r="CC273" s="22"/>
     </row>
-    <row r="274" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A274" s="17">
+    <row r="274" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A274" s="16">
         <v>270</v>
       </c>
       <c r="BY274" s="22"/>
       <c r="CA274" s="22"/>
       <c r="CC274" s="22"/>
     </row>
-    <row r="275" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A275" s="17">
+    <row r="275" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A275" s="16">
         <v>271</v>
       </c>
       <c r="BY275" s="22"/>
       <c r="CA275" s="22"/>
       <c r="CC275" s="22"/>
     </row>
-    <row r="276" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A276" s="17">
+    <row r="276" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A276" s="16">
         <v>272</v>
       </c>
       <c r="BY276" s="22"/>
       <c r="CA276" s="22"/>
       <c r="CC276" s="22"/>
     </row>
-    <row r="277" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A277" s="17">
+    <row r="277" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A277" s="16">
         <v>273</v>
       </c>
       <c r="BY277" s="22"/>
       <c r="CA277" s="22"/>
       <c r="CC277" s="22"/>
     </row>
-    <row r="278" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A278" s="17">
+    <row r="278" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A278" s="16">
         <v>274</v>
       </c>
       <c r="BY278" s="22"/>
       <c r="CA278" s="22"/>
       <c r="CC278" s="22"/>
     </row>
-    <row r="279" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A279" s="17">
+    <row r="279" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A279" s="16">
         <v>275</v>
       </c>
       <c r="BY279" s="22"/>
       <c r="CA279" s="22"/>
       <c r="CC279" s="22"/>
     </row>
-    <row r="280" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A280" s="17">
+    <row r="280" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A280" s="16">
         <v>276</v>
       </c>
       <c r="BY280" s="22"/>
       <c r="CA280" s="22"/>
       <c r="CC280" s="22"/>
     </row>
-    <row r="281" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A281" s="17">
+    <row r="281" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A281" s="16">
         <v>277</v>
       </c>
       <c r="BY281" s="22"/>
       <c r="CA281" s="22"/>
       <c r="CC281" s="22"/>
     </row>
-    <row r="282" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A282" s="17">
+    <row r="282" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A282" s="16">
         <v>278</v>
       </c>
       <c r="BY282" s="22"/>
       <c r="CA282" s="22"/>
       <c r="CC282" s="22"/>
     </row>
-    <row r="283" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A283" s="17">
+    <row r="283" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A283" s="16">
         <v>279</v>
       </c>
       <c r="BY283" s="22"/>
       <c r="CA283" s="22"/>
       <c r="CC283" s="22"/>
     </row>
-    <row r="284" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="17">
+    <row r="284" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A284" s="16">
         <v>280</v>
       </c>
       <c r="BY284" s="22"/>
       <c r="CA284" s="22"/>
       <c r="CC284" s="22"/>
     </row>
-    <row r="285" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A285" s="17">
+    <row r="285" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A285" s="16">
         <v>281</v>
       </c>
       <c r="BY285" s="22"/>
       <c r="CA285" s="22"/>
       <c r="CC285" s="22"/>
     </row>
-    <row r="286" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="17">
+    <row r="286" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A286" s="16">
         <v>282</v>
       </c>
       <c r="BY286" s="22"/>
       <c r="CA286" s="22"/>
       <c r="CC286" s="22"/>
     </row>
-    <row r="287" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A287" s="17">
+    <row r="287" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A287" s="16">
         <v>283</v>
       </c>
       <c r="BY287" s="22"/>
       <c r="CA287" s="22"/>
       <c r="CC287" s="22"/>
     </row>
-    <row r="288" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A288" s="17">
+    <row r="288" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A288" s="16">
         <v>284</v>
       </c>
       <c r="BY288" s="22"/>
       <c r="CA288" s="22"/>
       <c r="CC288" s="22"/>
     </row>
-    <row r="289" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A289" s="17">
+    <row r="289" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A289" s="16">
         <v>285</v>
       </c>
       <c r="BY289" s="22"/>
       <c r="CA289" s="22"/>
       <c r="CC289" s="22"/>
     </row>
-    <row r="290" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A290" s="17">
+    <row r="290" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A290" s="16">
         <v>286</v>
       </c>
       <c r="BY290" s="22"/>
       <c r="CA290" s="22"/>
       <c r="CC290" s="22"/>
     </row>
-    <row r="291" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A291" s="17">
+    <row r="291" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A291" s="16">
         <v>287</v>
       </c>
       <c r="BY291" s="22"/>
       <c r="CA291" s="22"/>
       <c r="CC291" s="22"/>
     </row>
-    <row r="292" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A292" s="17">
+    <row r="292" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="16">
         <v>288</v>
       </c>
       <c r="BY292" s="22"/>
       <c r="CA292" s="22"/>
       <c r="CC292" s="22"/>
     </row>
-    <row r="293" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A293" s="17">
+    <row r="293" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A293" s="16">
         <v>289</v>
       </c>
       <c r="BY293" s="22"/>
       <c r="CA293" s="22"/>
       <c r="CC293" s="22"/>
     </row>
-    <row r="294" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="17">
+    <row r="294" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A294" s="16">
         <v>290</v>
       </c>
       <c r="BY294" s="22"/>
       <c r="CA294" s="22"/>
       <c r="CC294" s="22"/>
     </row>
-    <row r="295" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="17">
+    <row r="295" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A295" s="16">
         <v>291</v>
       </c>
       <c r="BY295" s="22"/>
       <c r="CA295" s="22"/>
       <c r="CC295" s="22"/>
     </row>
-    <row r="296" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="17">
+    <row r="296" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A296" s="16">
         <v>292</v>
       </c>
       <c r="BY296" s="22"/>
       <c r="CA296" s="22"/>
       <c r="CC296" s="22"/>
     </row>
-    <row r="297" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A297" s="17">
+    <row r="297" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A297" s="16">
         <v>293</v>
       </c>
       <c r="BY297" s="22"/>
       <c r="CA297" s="22"/>
       <c r="CC297" s="22"/>
     </row>
-    <row r="298" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A298" s="17">
+    <row r="298" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A298" s="16">
         <v>294</v>
       </c>
       <c r="BY298" s="22"/>
       <c r="CA298" s="22"/>
       <c r="CC298" s="22"/>
     </row>
-    <row r="299" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="17">
+    <row r="299" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A299" s="16">
         <v>295</v>
       </c>
       <c r="BY299" s="22"/>
       <c r="CA299" s="22"/>
       <c r="CC299" s="22"/>
     </row>
-    <row r="300" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A300" s="17">
+    <row r="300" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="16">
         <v>296</v>
       </c>
       <c r="BY300" s="22"/>
       <c r="CA300" s="22"/>
       <c r="CC300" s="22"/>
     </row>
-    <row r="301" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A301" s="17">
+    <row r="301" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A301" s="16">
         <v>297</v>
       </c>
       <c r="BY301" s="22"/>
       <c r="CA301" s="22"/>
       <c r="CC301" s="22"/>
     </row>
-    <row r="302" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A302" s="17">
+    <row r="302" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A302" s="16">
         <v>298</v>
       </c>
       <c r="BY302" s="22"/>
       <c r="CA302" s="22"/>
       <c r="CC302" s="22"/>
     </row>
-    <row r="303" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A303" s="17">
+    <row r="303" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A303" s="16">
         <v>299</v>
       </c>
       <c r="BY303" s="22"/>
       <c r="CA303" s="22"/>
       <c r="CC303" s="22"/>
     </row>
-    <row r="304" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A304" s="17">
+    <row r="304" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A304" s="16">
         <v>300</v>
       </c>
       <c r="BY304" s="22"/>
       <c r="CA304" s="22"/>
       <c r="CC304" s="22"/>
     </row>
-    <row r="305" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A305" s="17">
+    <row r="305" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A305" s="16">
         <v>301</v>
       </c>
       <c r="BY305" s="22"/>
       <c r="CA305" s="22"/>
       <c r="CC305" s="22"/>
     </row>
-    <row r="306" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A306" s="17">
+    <row r="306" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A306" s="16">
         <v>302</v>
       </c>
       <c r="BY306" s="22"/>
       <c r="CA306" s="22"/>
       <c r="CC306" s="22"/>
     </row>
-    <row r="307" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A307" s="17">
+    <row r="307" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A307" s="16">
         <v>303</v>
       </c>
       <c r="BY307" s="22"/>
       <c r="CA307" s="22"/>
       <c r="CC307" s="22"/>
     </row>
-    <row r="308" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A308" s="17">
+    <row r="308" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A308" s="16">
         <v>304</v>
       </c>
       <c r="BY308" s="22"/>
       <c r="CA308" s="22"/>
       <c r="CC308" s="22"/>
     </row>
-    <row r="309" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A309" s="17">
+    <row r="309" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A309" s="16">
         <v>305</v>
       </c>
       <c r="BY309" s="22"/>
       <c r="CA309" s="22"/>
       <c r="CC309" s="22"/>
     </row>
-    <row r="310" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A310" s="17">
+    <row r="310" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A310" s="16">
         <v>306</v>
       </c>
       <c r="BY310" s="22"/>
       <c r="CA310" s="22"/>
       <c r="CC310" s="22"/>
     </row>
-    <row r="311" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A311" s="17">
+    <row r="311" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A311" s="16">
         <v>307</v>
       </c>
       <c r="BY311" s="22"/>
       <c r="CA311" s="22"/>
       <c r="CC311" s="22"/>
     </row>
-    <row r="312" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A312" s="17">
+    <row r="312" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A312" s="16">
         <v>308</v>
       </c>
       <c r="BY312" s="22"/>
       <c r="CA312" s="22"/>
       <c r="CC312" s="22"/>
     </row>
-    <row r="313" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A313" s="17">
+    <row r="313" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A313" s="16">
         <v>309</v>
       </c>
       <c r="BY313" s="22"/>
       <c r="CA313" s="22"/>
       <c r="CC313" s="22"/>
     </row>
-    <row r="314" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A314" s="17">
+    <row r="314" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A314" s="16">
         <v>310</v>
       </c>
       <c r="BY314" s="22"/>
       <c r="CA314" s="22"/>
       <c r="CC314" s="22"/>
     </row>
-    <row r="315" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A315" s="17">
+    <row r="315" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A315" s="16">
         <v>311</v>
       </c>
       <c r="BY315" s="22"/>
       <c r="CA315" s="22"/>
       <c r="CC315" s="22"/>
     </row>
-    <row r="316" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="17">
+    <row r="316" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A316" s="16">
         <v>312</v>
       </c>
       <c r="BY316" s="22"/>
       <c r="CA316" s="22"/>
       <c r="CC316" s="22"/>
     </row>
-    <row r="317" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A317" s="17">
+    <row r="317" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A317" s="16">
         <v>313</v>
       </c>
       <c r="BY317" s="22"/>
       <c r="CA317" s="22"/>
       <c r="CC317" s="22"/>
     </row>
-    <row r="318" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A318" s="17">
+    <row r="318" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A318" s="16">
         <v>314</v>
       </c>
       <c r="BY318" s="22"/>
       <c r="CA318" s="22"/>
       <c r="CC318" s="22"/>
     </row>
-    <row r="319" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A319" s="17">
+    <row r="319" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A319" s="16">
         <v>315</v>
       </c>
       <c r="BY319" s="22"/>
       <c r="CA319" s="22"/>
       <c r="CC319" s="22"/>
     </row>
-    <row r="320" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A320" s="17">
+    <row r="320" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A320" s="16">
         <v>316</v>
       </c>
       <c r="BY320" s="22"/>
       <c r="CA320" s="22"/>
       <c r="CC320" s="22"/>
     </row>
-    <row r="321" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A321" s="17">
+    <row r="321" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A321" s="16">
         <v>317</v>
       </c>
       <c r="BY321" s="22"/>
       <c r="CA321" s="22"/>
       <c r="CC321" s="22"/>
     </row>
-    <row r="322" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A322" s="17">
+    <row r="322" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A322" s="16">
         <v>318</v>
       </c>
       <c r="BY322" s="22"/>
       <c r="CA322" s="22"/>
       <c r="CC322" s="22"/>
     </row>
-    <row r="323" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A323" s="17">
+    <row r="323" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A323" s="16">
         <v>319</v>
       </c>
       <c r="BY323" s="22"/>
       <c r="CA323" s="22"/>
       <c r="CC323" s="22"/>
     </row>
-    <row r="324" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="17">
+    <row r="324" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A324" s="16">
         <v>320</v>
       </c>
       <c r="BY324" s="22"/>
       <c r="CA324" s="22"/>
       <c r="CC324" s="22"/>
     </row>
-    <row r="325" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A325" s="17">
+    <row r="325" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A325" s="16">
         <v>321</v>
       </c>
       <c r="BY325" s="22"/>
       <c r="CA325" s="22"/>
       <c r="CC325" s="22"/>
     </row>
-    <row r="326" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="17">
+    <row r="326" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A326" s="16">
         <v>322</v>
       </c>
       <c r="BY326" s="22"/>
       <c r="CA326" s="22"/>
       <c r="CC326" s="22"/>
     </row>
-    <row r="327" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="17">
+    <row r="327" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A327" s="16">
         <v>323</v>
       </c>
       <c r="BY327" s="22"/>
       <c r="CA327" s="22"/>
       <c r="CC327" s="22"/>
     </row>
-    <row r="328" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A328" s="17">
+    <row r="328" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A328" s="16">
         <v>324</v>
       </c>
       <c r="BY328" s="22"/>
       <c r="CA328" s="22"/>
       <c r="CC328" s="22"/>
     </row>
-    <row r="329" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A329" s="17">
+    <row r="329" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A329" s="16">
         <v>325</v>
       </c>
       <c r="BY329" s="22"/>
       <c r="CA329" s="22"/>
       <c r="CC329" s="22"/>
     </row>
-    <row r="330" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A330" s="17">
+    <row r="330" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A330" s="16">
         <v>326</v>
       </c>
       <c r="BY330" s="22"/>
       <c r="CA330" s="22"/>
       <c r="CC330" s="22"/>
     </row>
-    <row r="331" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A331" s="17">
+    <row r="331" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A331" s="16">
         <v>327</v>
       </c>
       <c r="BY331" s="22"/>
       <c r="CA331" s="22"/>
       <c r="CC331" s="22"/>
     </row>
-    <row r="332" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A332" s="17">
+    <row r="332" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A332" s="16">
         <v>328</v>
       </c>
       <c r="BY332" s="22"/>
       <c r="CA332" s="22"/>
       <c r="CC332" s="22"/>
     </row>
-    <row r="333" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A333" s="17">
+    <row r="333" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A333" s="16">
         <v>329</v>
       </c>
       <c r="BY333" s="22"/>
       <c r="CA333" s="22"/>
       <c r="CC333" s="22"/>
     </row>
-    <row r="334" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A334" s="17">
+    <row r="334" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A334" s="16">
         <v>330</v>
       </c>
       <c r="BY334" s="22"/>
       <c r="CA334" s="22"/>
       <c r="CC334" s="22"/>
     </row>
-    <row r="335" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A335" s="17">
+    <row r="335" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A335" s="16">
         <v>331</v>
       </c>
       <c r="BY335" s="22"/>
       <c r="CA335" s="22"/>
       <c r="CC335" s="22"/>
     </row>
-    <row r="336" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A336" s="17">
+    <row r="336" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A336" s="16">
         <v>332</v>
       </c>
       <c r="BY336" s="22"/>
       <c r="CA336" s="22"/>
       <c r="CC336" s="22"/>
     </row>
-    <row r="337" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A337" s="17">
+    <row r="337" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A337" s="16">
         <v>333</v>
       </c>
       <c r="BY337" s="22"/>
       <c r="CA337" s="22"/>
       <c r="CC337" s="22"/>
     </row>
-    <row r="338" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A338" s="17">
+    <row r="338" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A338" s="16">
         <v>334</v>
       </c>
       <c r="BY338" s="22"/>
       <c r="CA338" s="22"/>
       <c r="CC338" s="22"/>
     </row>
-    <row r="339" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A339" s="17">
+    <row r="339" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A339" s="16">
         <v>335</v>
       </c>
       <c r="BY339" s="22"/>
       <c r="CA339" s="22"/>
       <c r="CC339" s="22"/>
     </row>
-    <row r="340" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A340" s="17">
+    <row r="340" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A340" s="16">
         <v>336</v>
       </c>
       <c r="BY340" s="22"/>
       <c r="CA340" s="22"/>
       <c r="CC340" s="22"/>
     </row>
-    <row r="341" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A341" s="17">
+    <row r="341" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A341" s="16">
         <v>337</v>
       </c>
       <c r="BY341" s="22"/>
       <c r="CA341" s="22"/>
       <c r="CC341" s="22"/>
     </row>
-    <row r="342" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A342" s="17">
+    <row r="342" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A342" s="16">
         <v>338</v>
       </c>
       <c r="BY342" s="22"/>
       <c r="CA342" s="22"/>
       <c r="CC342" s="22"/>
     </row>
-    <row r="343" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="17">
+    <row r="343" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A343" s="16">
         <v>339</v>
       </c>
       <c r="BY343" s="22"/>
       <c r="CA343" s="22"/>
       <c r="CC343" s="22"/>
     </row>
-    <row r="344" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A344" s="17">
+    <row r="344" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A344" s="16">
         <v>340</v>
       </c>
       <c r="BY344" s="22"/>
       <c r="CA344" s="22"/>
       <c r="CC344" s="22"/>
     </row>
-    <row r="345" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A345" s="17">
+    <row r="345" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A345" s="16">
         <v>341</v>
       </c>
       <c r="BY345" s="22"/>
       <c r="CA345" s="22"/>
       <c r="CC345" s="22"/>
     </row>
-    <row r="346" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="17">
+    <row r="346" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A346" s="16">
         <v>342</v>
       </c>
       <c r="BY346" s="22"/>
       <c r="CA346" s="22"/>
       <c r="CC346" s="22"/>
     </row>
-    <row r="347" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A347" s="17">
+    <row r="347" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A347" s="16">
         <v>343</v>
       </c>
       <c r="BY347" s="22"/>
       <c r="CA347" s="22"/>
       <c r="CC347" s="22"/>
     </row>
-    <row r="348" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="17">
+    <row r="348" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A348" s="16">
         <v>344</v>
       </c>
       <c r="BY348" s="22"/>
       <c r="CA348" s="22"/>
       <c r="CC348" s="22"/>
     </row>
-    <row r="349" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A349" s="17">
+    <row r="349" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A349" s="16">
         <v>345</v>
       </c>
       <c r="BY349" s="22"/>
       <c r="CA349" s="22"/>
       <c r="CC349" s="22"/>
     </row>
-    <row r="350" spans="1:81" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A350" s="17">
+    <row r="350" spans="1:81" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A350" s="16">
         <v>346</v>
       </c>
       <c r="BY350" s="22"/>
@@ -4541,6 +4538,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="AA1:AA3"/>
     <mergeCell ref="CE1:CE3"/>
     <mergeCell ref="CG1:CG3"/>
     <mergeCell ref="CH1:CH3"/>
@@ -4548,7 +4546,6 @@
     <mergeCell ref="BY1:BY3"/>
     <mergeCell ref="CA1:CA3"/>
     <mergeCell ref="CC1:CC3"/>
-    <mergeCell ref="AA1:AA3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>